<commit_message>
Fixed a large number of bugs when importing tables. Added un region definitions.
</commit_message>
<xml_diff>
--- a/tests/common/truthset.xlsx
+++ b/tests/common/truthset.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>regionCode</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>doublingYear</t>
+  </si>
+  <si>
+    <t>indexYear</t>
   </si>
 </sst>
 </file>
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY17"/>
+  <dimension ref="A1:AY18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2969,7 +2972,7 @@
         <v>57.995725081221607</v>
       </c>
       <c r="L16">
-        <f t="shared" ref="K16:AY16" si="11">LOG(2)/LOG(L15)</f>
+        <f t="shared" ref="L16:AY16" si="11">LOG(2)/LOG(L15)</f>
         <v>69.066194403895082</v>
       </c>
       <c r="M16">
@@ -3300,6 +3303,183 @@
       <c r="AY17">
         <f t="shared" si="12"/>
         <v>2085.3122852034335</v>
+      </c>
+    </row>
+    <row r="18" spans="4:51" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18">
+        <f>(I4 - $AC$4)/$AC$4</f>
+        <v>-0.1936761413551733</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ref="J18:AY18" si="13">(J4 - $AC$4)/$AC$4</f>
+        <v>-0.18554991923371214</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="13"/>
+        <v>-0.17771417235809223</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="13"/>
+        <v>-0.17020786691982884</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="13"/>
+        <v>-0.16291056196332926</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="13"/>
+        <v>-0.15543968033553432</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="13"/>
+        <v>-0.14772791679655398</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="13"/>
+        <v>-0.14008345849746365</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="13"/>
+        <v>-0.13222999971660951</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="13"/>
+        <v>-0.12401876045002409</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="13"/>
+        <v>-0.11423824637968658</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="13"/>
+        <v>-0.1023889817779919</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="13"/>
+        <v>-9.0398021934423436E-2</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="13"/>
+        <v>-7.8463740187604394E-2</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="13"/>
+        <v>-6.7202510839686008E-2</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="13"/>
+        <v>-5.6104231019922249E-2</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="13"/>
+        <v>-4.5041375010627147E-2</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="13"/>
+        <v>-3.3560518037804292E-2</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="13"/>
+        <v>-2.2224898687902062E-2</v>
+      </c>
+      <c r="AB18">
+        <f t="shared" si="13"/>
+        <v>-1.0984923626264629E-2</v>
+      </c>
+      <c r="AC18">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="13"/>
+        <v>1.0343752656785785E-2</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" si="13"/>
+        <v>2.0273046731090771E-2</v>
+      </c>
+      <c r="AF18">
+        <f t="shared" si="13"/>
+        <v>2.9887068892226597E-2</v>
+      </c>
+      <c r="AG18">
+        <f t="shared" si="13"/>
+        <v>3.9295632952645453E-2</v>
+      </c>
+      <c r="AH18">
+        <f t="shared" si="13"/>
+        <v>4.8952163686343413E-2</v>
+      </c>
+      <c r="AI18">
+        <f t="shared" si="13"/>
+        <v>5.892396633321053E-2</v>
+      </c>
+      <c r="AJ18">
+        <f t="shared" si="13"/>
+        <v>6.9455465185479071E-2</v>
+      </c>
+      <c r="AK18">
+        <f t="shared" si="13"/>
+        <v>7.9427267832346188E-2</v>
+      </c>
+      <c r="AL18">
+        <f t="shared" si="13"/>
+        <v>8.8835831892765046E-2</v>
+      </c>
+      <c r="AM18">
+        <f t="shared" si="13"/>
+        <v>9.7273783546348511E-2</v>
+      </c>
+      <c r="AN18">
+        <f t="shared" si="13"/>
+        <v>0.1052901918553575</v>
+      </c>
+      <c r="AO18">
+        <f t="shared" si="13"/>
+        <v>0.11331368492646017</v>
+      </c>
+      <c r="AP18">
+        <f t="shared" si="13"/>
+        <v>0.1210785841811432</v>
+      </c>
+      <c r="AQ18">
+        <f t="shared" si="13"/>
+        <v>0.12927211154249441</v>
+      </c>
+      <c r="AR18">
+        <f t="shared" si="13"/>
+        <v>0.13738770652081503</v>
+      </c>
+      <c r="AS18">
+        <f t="shared" si="13"/>
+        <v>0.14524470768271602</v>
+      </c>
+      <c r="AT18">
+        <f t="shared" si="13"/>
+        <v>0.15389874458015701</v>
+      </c>
+      <c r="AU18">
+        <f t="shared" si="13"/>
+        <v>0.16276532434040866</v>
+      </c>
+      <c r="AV18">
+        <f t="shared" si="13"/>
+        <v>0.17169920934055036</v>
+      </c>
+      <c r="AW18">
+        <f t="shared" si="13"/>
+        <v>0.18070039958058209</v>
+      </c>
+      <c r="AX18">
+        <f t="shared" si="13"/>
+        <v>0.18976889506050387</v>
+      </c>
+      <c r="AY18">
+        <f t="shared" si="13"/>
+        <v>0.19891178054240938</v>
       </c>
     </row>
   </sheetData>

</xml_diff>